<commit_message>
Add Soldier Cat & 엑셀 PPT 수정
</commit_message>
<xml_diff>
--- a/Cat Defense Design.xlsx
+++ b/Cat Defense Design.xlsx
@@ -507,11 +507,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>